<commit_message>
make x axis fit correctly
</commit_message>
<xml_diff>
--- a/client/data/Pensions calculator.xlsx
+++ b/client/data/Pensions calculator.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="80" windowWidth="24920" windowHeight="17500"/>
+    <workbookView xWindow="120" yWindow="80" windowWidth="30520" windowHeight="22500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -192,121 +192,121 @@
                   <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4020.0</c:v>
+                  <c:v>4110.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6060.2</c:v>
+                  <c:v>6336.05</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8120.802</c:v>
+                  <c:v>8684.532749999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10202.01002</c:v>
+                  <c:v>11162.18205125</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12304.0301202</c:v>
+                  <c:v>13776.10206406875</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14427.070421402</c:v>
+                  <c:v>16533.78767759253</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16571.34112561602</c:v>
+                  <c:v>19443.14599986011</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18737.05453687218</c:v>
+                  <c:v>22512.51902985242</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20924.4250822409</c:v>
+                  <c:v>25750.7075764943</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>23133.66933306331</c:v>
+                  <c:v>29166.99649320148</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>25365.00602639394</c:v>
+                  <c:v>32771.18130032756</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>27618.65608665788</c:v>
+                  <c:v>36573.59627184557</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>29894.84264752446</c:v>
+                  <c:v>40585.14406679707</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>32193.79107399971</c:v>
+                  <c:v>44817.3269904709</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>34515.7289847397</c:v>
+                  <c:v>49282.2799749468</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>36860.8862745871</c:v>
+                  <c:v>53992.80537356887</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>39229.49513733297</c:v>
+                  <c:v>58962.40966911516</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>41621.79008870631</c:v>
+                  <c:v>64205.34220091648</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44038.00798959337</c:v>
+                  <c:v>69736.63602196689</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>46478.3880694893</c:v>
+                  <c:v>75572.15100317506</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>48943.1719501842</c:v>
+                  <c:v>81728.6193083497</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>51432.60366968605</c:v>
+                  <c:v>88223.69337030891</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>53946.92970638291</c:v>
+                  <c:v>95075.9965056759</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>56486.39900344673</c:v>
+                  <c:v>102305.1763134881</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>59051.2629934812</c:v>
+                  <c:v>109931.9610107299</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>61641.77562341601</c:v>
+                  <c:v>117978.21886632</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>64258.19337965017</c:v>
+                  <c:v>126467.0209039676</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>66900.77531344667</c:v>
+                  <c:v>135422.7070536859</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>69569.78306658114</c:v>
+                  <c:v>144870.9559416386</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>72265.48089724696</c:v>
+                  <c:v>154838.8585184287</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>74988.13570621943</c:v>
+                  <c:v>165354.9957369422</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>77738.01706328163</c:v>
+                  <c:v>176449.520502474</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>80515.39723391445</c:v>
+                  <c:v>188154.2441301101</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>83320.5512062536</c:v>
+                  <c:v>200502.7275572662</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>86153.75671831613</c:v>
+                  <c:v>213530.3775729158</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>89015.29428549929</c:v>
+                  <c:v>227274.5483394261</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>91905.44722835429</c:v>
+                  <c:v>241774.6484980946</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>94824.50170063783</c:v>
+                  <c:v>257072.2541654898</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>97772.74671764421</c:v>
+                  <c:v>273211.2281445917</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -464,8 +464,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2080596904"/>
-        <c:axId val="-2080588360"/>
+        <c:axId val="-2085674952"/>
+        <c:axId val="-2085703624"/>
       </c:areaChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -625,11 +625,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2080596904"/>
-        <c:axId val="-2080588360"/>
+        <c:axId val="-2085674952"/>
+        <c:axId val="-2085703624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2080596904"/>
+        <c:axId val="-2085674952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -664,7 +664,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080588360"/>
+        <c:crossAx val="-2085703624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -674,7 +674,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2080588360"/>
+        <c:axId val="-2085703624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -719,7 +719,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080596904"/>
+        <c:crossAx val="-2085674952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1137,7 +1137,7 @@
   <dimension ref="A1:C472"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1193,7 +1193,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="3">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C5">
         <v>0.02</v>
@@ -1205,7 +1205,7 @@
       </c>
       <c r="B6" s="3">
         <f>B4-B5</f>
-        <v>9.999999999999995E-3</v>
+        <v>5.5E-2</v>
       </c>
       <c r="C6">
         <f>C4-C5</f>
@@ -1218,7 +1218,7 @@
       </c>
       <c r="B7" s="3">
         <f>1+B6</f>
-        <v>1.01</v>
+        <v>1.0549999999999999</v>
       </c>
       <c r="C7">
         <f>1+C6</f>
@@ -1231,7 +1231,7 @@
       </c>
       <c r="B9" s="3">
         <f>(B7^B3-B7)/(B7-1)</f>
-        <v>47.886373358822112</v>
+        <v>135.60561407229602</v>
       </c>
       <c r="C9" s="3">
         <f>(C7^C3-C7)/(C7-1)</f>
@@ -1244,7 +1244,7 @@
       </c>
       <c r="B10" s="3">
         <f>B9*(B2)</f>
-        <v>95772.74671764423</v>
+        <v>271211.22814459202</v>
       </c>
       <c r="C10" s="3">
         <f>C9*(C2)</f>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="B11" s="3">
         <f>B10+B2:B2</f>
-        <v>97772.74671764423</v>
+        <v>273211.22814459202</v>
       </c>
       <c r="C11" s="3">
         <f>C10+C2:C2</f>
@@ -1299,7 +1299,7 @@
       </c>
       <c r="B15" s="3">
         <f>B14*B$7+B$2</f>
-        <v>4020</v>
+        <v>4110</v>
       </c>
       <c r="C15" s="3">
         <f>C14*C$7+C$2</f>
@@ -1312,7 +1312,7 @@
       </c>
       <c r="B16" s="3">
         <f t="shared" ref="B16:B32" si="0">B15*B$7+B$2</f>
-        <v>6060.2</v>
+        <v>6336.05</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" ref="C16:C32" si="1">C15*C$7+C$2</f>
@@ -1325,7 +1325,7 @@
       </c>
       <c r="B17" s="3">
         <f t="shared" si="0"/>
-        <v>8120.8019999999997</v>
+        <v>8684.5327499999985</v>
       </c>
       <c r="C17" s="3">
         <f t="shared" si="1"/>
@@ -1338,7 +1338,7 @@
       </c>
       <c r="B18" s="3">
         <f t="shared" si="0"/>
-        <v>10202.01002</v>
+        <v>11162.182051249998</v>
       </c>
       <c r="C18" s="3">
         <f t="shared" si="1"/>
@@ -1351,7 +1351,7 @@
       </c>
       <c r="B19" s="3">
         <f t="shared" si="0"/>
-        <v>12304.030120199999</v>
+        <v>13776.102064068747</v>
       </c>
       <c r="C19" s="3">
         <f t="shared" si="1"/>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="B20" s="3">
         <f t="shared" si="0"/>
-        <v>14427.070421401999</v>
+        <v>16533.787677592525</v>
       </c>
       <c r="C20" s="3">
         <f t="shared" si="1"/>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="B21" s="3">
         <f t="shared" si="0"/>
-        <v>16571.341125616018</v>
+        <v>19443.145999860113</v>
       </c>
       <c r="C21" s="3">
         <f t="shared" si="1"/>
@@ -1390,7 +1390,7 @@
       </c>
       <c r="B22" s="3">
         <f t="shared" si="0"/>
-        <v>18737.05453687218</v>
+        <v>22512.519029852418</v>
       </c>
       <c r="C22" s="3">
         <f t="shared" si="1"/>
@@ -1403,7 +1403,7 @@
       </c>
       <c r="B23" s="3">
         <f t="shared" si="0"/>
-        <v>20924.425082240901</v>
+        <v>25750.7075764943</v>
       </c>
       <c r="C23" s="3">
         <f t="shared" si="1"/>
@@ -1416,7 +1416,7 @@
       </c>
       <c r="B24" s="3">
         <f t="shared" si="0"/>
-        <v>23133.66933306331</v>
+        <v>29166.996493201485</v>
       </c>
       <c r="C24" s="3">
         <f t="shared" si="1"/>
@@ -1429,7 +1429,7 @@
       </c>
       <c r="B25" s="3">
         <f t="shared" si="0"/>
-        <v>25365.006026393941</v>
+        <v>32771.18130032756</v>
       </c>
       <c r="C25" s="3">
         <f t="shared" si="1"/>
@@ -1442,7 +1442,7 @@
       </c>
       <c r="B26" s="3">
         <f t="shared" si="0"/>
-        <v>27618.65608665788</v>
+        <v>36573.59627184557</v>
       </c>
       <c r="C26" s="3">
         <f t="shared" si="1"/>
@@ -1455,7 +1455,7 @@
       </c>
       <c r="B27" s="3">
         <f t="shared" si="0"/>
-        <v>29894.84264752446</v>
+        <v>40585.144066797075</v>
       </c>
       <c r="C27" s="3">
         <f t="shared" si="1"/>
@@ -1468,7 +1468,7 @@
       </c>
       <c r="B28" s="3">
         <f t="shared" si="0"/>
-        <v>32193.791073999706</v>
+        <v>44817.326990470909</v>
       </c>
       <c r="C28" s="3">
         <f t="shared" si="1"/>
@@ -1481,7 +1481,7 @@
       </c>
       <c r="B29" s="3">
         <f t="shared" si="0"/>
-        <v>34515.728984739704</v>
+        <v>49282.279974946803</v>
       </c>
       <c r="C29" s="3">
         <f t="shared" si="1"/>
@@ -1494,7 +1494,7 @@
       </c>
       <c r="B30" s="3">
         <f t="shared" si="0"/>
-        <v>36860.886274587101</v>
+        <v>53992.805373568874</v>
       </c>
       <c r="C30" s="3">
         <f t="shared" si="1"/>
@@ -1507,7 +1507,7 @@
       </c>
       <c r="B31" s="3">
         <f t="shared" si="0"/>
-        <v>39229.495137332975</v>
+        <v>58962.409669115157</v>
       </c>
       <c r="C31" s="3">
         <f t="shared" si="1"/>
@@ -1520,7 +1520,7 @@
       </c>
       <c r="B32" s="3">
         <f t="shared" si="0"/>
-        <v>41621.790088706308</v>
+        <v>64205.342200916486</v>
       </c>
       <c r="C32" s="3">
         <f t="shared" si="1"/>
@@ -1533,7 +1533,7 @@
       </c>
       <c r="B33" s="3">
         <f t="shared" ref="B33:B53" si="2">B32*B$7+B$2</f>
-        <v>44038.007989593374</v>
+        <v>69736.636021966886</v>
       </c>
       <c r="C33" s="3">
         <f t="shared" ref="C33:C53" si="3">C32*C$7+C$2</f>
@@ -1546,7 +1546,7 @@
       </c>
       <c r="B34" s="3">
         <f t="shared" si="2"/>
-        <v>46478.388069489309</v>
+        <v>75572.151003175066</v>
       </c>
       <c r="C34" s="3">
         <f t="shared" si="3"/>
@@ -1559,7 +1559,7 @@
       </c>
       <c r="B35" s="3">
         <f t="shared" si="2"/>
-        <v>48943.171950184202</v>
+        <v>81728.619308349691</v>
       </c>
       <c r="C35" s="3">
         <f t="shared" si="3"/>
@@ -1572,7 +1572,7 @@
       </c>
       <c r="B36" s="3">
         <f t="shared" si="2"/>
-        <v>51432.603669686046</v>
+        <v>88223.693370308916</v>
       </c>
       <c r="C36" s="3">
         <f t="shared" si="3"/>
@@ -1585,7 +1585,7 @@
       </c>
       <c r="B37" s="3">
         <f t="shared" si="2"/>
-        <v>53946.929706382907</v>
+        <v>95075.996505675896</v>
       </c>
       <c r="C37" s="3">
         <f t="shared" si="3"/>
@@ -1598,7 +1598,7 @@
       </c>
       <c r="B38" s="3">
         <f t="shared" si="2"/>
-        <v>56486.399003446735</v>
+        <v>102305.17631348806</v>
       </c>
       <c r="C38" s="3">
         <f t="shared" si="3"/>
@@ -1611,7 +1611,7 @@
       </c>
       <c r="B39" s="3">
         <f t="shared" si="2"/>
-        <v>59051.262993481199</v>
+        <v>109931.96101072989</v>
       </c>
       <c r="C39" s="3">
         <f t="shared" si="3"/>
@@ -1624,7 +1624,7 @@
       </c>
       <c r="B40" s="3">
         <f t="shared" si="2"/>
-        <v>61641.775623416012</v>
+        <v>117978.21886632004</v>
       </c>
       <c r="C40" s="3">
         <f t="shared" si="3"/>
@@ -1637,7 +1637,7 @@
       </c>
       <c r="B41" s="3">
         <f t="shared" si="2"/>
-        <v>64258.193379650169</v>
+        <v>126467.02090396763</v>
       </c>
       <c r="C41" s="3">
         <f t="shared" si="3"/>
@@ -1650,7 +1650,7 @@
       </c>
       <c r="B42" s="3">
         <f t="shared" si="2"/>
-        <v>66900.775313446677</v>
+        <v>135422.70705368585</v>
       </c>
       <c r="C42" s="3">
         <f t="shared" si="3"/>
@@ -1663,7 +1663,7 @@
       </c>
       <c r="B43" s="3">
         <f t="shared" si="2"/>
-        <v>69569.783066581149</v>
+        <v>144870.95594163856</v>
       </c>
       <c r="C43" s="3">
         <f t="shared" si="3"/>
@@ -1676,7 +1676,7 @@
       </c>
       <c r="B44" s="3">
         <f t="shared" si="2"/>
-        <v>72265.480897246962</v>
+        <v>154838.85851842866</v>
       </c>
       <c r="C44" s="3">
         <f t="shared" si="3"/>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="B45" s="3">
         <f t="shared" si="2"/>
-        <v>74988.135706219429</v>
+        <v>165354.99573694222</v>
       </c>
       <c r="C45" s="3">
         <f t="shared" si="3"/>
@@ -1702,7 +1702,7 @@
       </c>
       <c r="B46" s="3">
         <f t="shared" si="2"/>
-        <v>77738.01706328163</v>
+        <v>176449.52050247404</v>
       </c>
       <c r="C46" s="3">
         <f t="shared" si="3"/>
@@ -1715,7 +1715,7 @@
       </c>
       <c r="B47" s="3">
         <f t="shared" si="2"/>
-        <v>80515.397233914453</v>
+        <v>188154.24413011011</v>
       </c>
       <c r="C47" s="3">
         <f t="shared" si="3"/>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="B48" s="3">
         <f t="shared" si="2"/>
-        <v>83320.5512062536</v>
+        <v>200502.72755726616</v>
       </c>
       <c r="C48" s="3">
         <f t="shared" si="3"/>
@@ -1741,7 +1741,7 @@
       </c>
       <c r="B49" s="3">
         <f t="shared" si="2"/>
-        <v>86153.75671831613</v>
+        <v>213530.37757291578</v>
       </c>
       <c r="C49" s="3">
         <f t="shared" si="3"/>
@@ -1754,7 +1754,7 @@
       </c>
       <c r="B50" s="3">
         <f t="shared" si="2"/>
-        <v>89015.294285499287</v>
+        <v>227274.54833942614</v>
       </c>
       <c r="C50" s="3">
         <f t="shared" si="3"/>
@@ -1767,7 +1767,7 @@
       </c>
       <c r="B51" s="3">
         <f t="shared" si="2"/>
-        <v>91905.447228354285</v>
+        <v>241774.64849809455</v>
       </c>
       <c r="C51" s="3">
         <f t="shared" si="3"/>
@@ -1780,7 +1780,7 @@
       </c>
       <c r="B52" s="3">
         <f t="shared" si="2"/>
-        <v>94824.501700637833</v>
+        <v>257072.25416548975</v>
       </c>
       <c r="C52" s="3">
         <f t="shared" si="3"/>
@@ -1793,7 +1793,7 @@
       </c>
       <c r="B53" s="3">
         <f t="shared" si="2"/>
-        <v>97772.746717644215</v>
+        <v>273211.22814459167</v>
       </c>
       <c r="C53" s="3">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Style changes to main paragraphs
Text amendmends also
</commit_message>
<xml_diff>
--- a/client/data/Pensions calculator.xlsx
+++ b/client/data/Pensions calculator.xlsx
@@ -491,8 +491,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2079131096"/>
-        <c:axId val="-2079127160"/>
+        <c:axId val="-2113121576"/>
+        <c:axId val="-2113118200"/>
       </c:areaChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -652,11 +652,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2079131096"/>
-        <c:axId val="-2079127160"/>
+        <c:axId val="-2113121576"/>
+        <c:axId val="-2113118200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2079131096"/>
+        <c:axId val="-2113121576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -691,7 +691,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079127160"/>
+        <c:crossAx val="-2113118200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -701,7 +701,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2079127160"/>
+        <c:axId val="-2113118200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -746,7 +746,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079131096"/>
+        <c:crossAx val="-2113121576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1164,7 +1164,7 @@
   <dimension ref="A1:C473"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>

</xml_diff>